<commit_message>
Correcting power curve: was overestimating power
Speed: 29kmh
Measured Power using the Elite App: 176 watts
Calculated Power using the cubic-polynomial: 195 watts (overestimating bzy 20 watts=

Switched to quartic-polynomial with lower error residual
</commit_message>
<xml_diff>
--- a/resources/TrainerPower.xlsx
+++ b/resources/TrainerPower.xlsx
@@ -526,7 +526,7 @@
           <c:x val="0.311086"/>
           <c:y val="0"/>
           <c:w val="0.377828"/>
-          <c:h val="0.121536"/>
+          <c:h val="0.123074"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -543,9 +543,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.189136"/>
-          <c:y val="0.121536"/>
+          <c:y val="0.123074"/>
           <c:w val="0.786554"/>
-          <c:h val="0.681578"/>
+          <c:h val="0.677705"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -561,10 +561,9 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln w="47625" cap="flat">
+            <a:ln w="12700" cap="flat">
               <a:noFill/>
-              <a:prstDash val="solid"/>
-              <a:round/>
+              <a:miter lim="400000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -629,7 +628,7 @@
               </a:effectLst>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="3"/>
+            <c:order val="4"/>
             <c:forward val="0"/>
             <c:backward val="0"/>
             <c:dispRSqr val="0"/>
@@ -656,7 +655,25 @@
                         </a:solidFill>
                         <a:latin typeface="Helvetica Neue"/>
                       </a:rPr>
-                      <a:t>y = -0,0009x</a:t>
+                      <a:t>y = 4,622E-5x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" baseline="33200" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t>4</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t> - 0,0054x</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr b="0" baseline="33200" i="0" strike="noStrike" sz="1000" u="none">
@@ -674,7 +691,7 @@
                         </a:solidFill>
                         <a:latin typeface="Helvetica Neue"/>
                       </a:rPr>
-                      <a:t> + 0,1173x</a:t>
+                      <a:t> + 0,2555x</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr b="0" baseline="33200" i="0" strike="noStrike" sz="1000" u="none">
@@ -692,7 +709,7 @@
                         </a:solidFill>
                         <a:latin typeface="Helvetica Neue"/>
                       </a:rPr>
-                      <a:t> + 3,437x - 1,236</a:t>
+                      <a:t> + 2,088x - 0,2197</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -1004,13 +1021,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>109270</xdr:rowOff>
+      <xdr:rowOff>175315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>511098</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>52628</xdr:rowOff>
+      <xdr:colOff>511100</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>53628</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1018,8 +1035,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="-409499" y="13041045"/>
-        <a:ext cx="5489499" cy="4492499"/>
+        <a:off x="-1" y="13041050"/>
+        <a:ext cx="5489501" cy="4436344"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2058,7 +2075,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2956,6 +2973,286 @@
       <c r="K59" s="26"/>
       <c r="L59" s="27"/>
     </row>
+    <row r="60" ht="14.7" customHeight="1">
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="7"/>
+    </row>
+    <row r="61" ht="14.7" customHeight="1">
+      <c r="A61" s="24"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="12"/>
+    </row>
+    <row r="62" ht="14.7" customHeight="1">
+      <c r="A62" s="24"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="12"/>
+    </row>
+    <row r="63" ht="14.7" customHeight="1">
+      <c r="A63" s="24"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="12"/>
+    </row>
+    <row r="64" ht="14.7" customHeight="1">
+      <c r="A64" s="24"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="12"/>
+    </row>
+    <row r="65" ht="14.7" customHeight="1">
+      <c r="A65" s="24"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="12"/>
+    </row>
+    <row r="66" ht="14.7" customHeight="1">
+      <c r="A66" s="24"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="12"/>
+    </row>
+    <row r="67" ht="14.7" customHeight="1">
+      <c r="A67" s="24"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="12"/>
+    </row>
+    <row r="68" ht="14.7" customHeight="1">
+      <c r="A68" s="24"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="12"/>
+    </row>
+    <row r="69" ht="14.7" customHeight="1">
+      <c r="A69" s="24"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="12"/>
+    </row>
+    <row r="70" ht="14.7" customHeight="1">
+      <c r="A70" s="24"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="12"/>
+    </row>
+    <row r="71" ht="14.7" customHeight="1">
+      <c r="A71" s="24"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="12"/>
+    </row>
+    <row r="72" ht="14.7" customHeight="1">
+      <c r="A72" s="24"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="12"/>
+    </row>
+    <row r="73" ht="14.7" customHeight="1">
+      <c r="A73" s="24"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+      <c r="L73" s="12"/>
+    </row>
+    <row r="74" ht="14.7" customHeight="1">
+      <c r="A74" s="24"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="11"/>
+      <c r="L74" s="12"/>
+    </row>
+    <row r="75" ht="14.7" customHeight="1">
+      <c r="A75" s="24"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="11"/>
+      <c r="L75" s="12"/>
+    </row>
+    <row r="76" ht="14.7" customHeight="1">
+      <c r="A76" s="24"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="11"/>
+      <c r="L76" s="12"/>
+    </row>
+    <row r="77" ht="14.7" customHeight="1">
+      <c r="A77" s="24"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" ht="14.7" customHeight="1">
+      <c r="A78" s="24"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" ht="14.7" customHeight="1">
+      <c r="A79" s="25"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="26"/>
+      <c r="L79" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>

</xml_diff>